<commit_message>
Better vis for sales per state?
</commit_message>
<xml_diff>
--- a/cstate_per_category.xlsx
+++ b/cstate_per_category.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruchi\Desktop\cw53\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr19aal\cw53\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F2915D7-33E8-4595-9B70-016BEFE4D4BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="maranhao" sheetId="1" r:id="rId1"/>
     <sheet name="GAIOS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -182,7 +180,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.00"/>
   </numFmts>
@@ -389,8 +387,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Sheet1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal_Sheet2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal_Sheet1" xfId="1"/>
+    <cellStyle name="Normal_Sheet2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -449,6 +447,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -825,7 +824,7 @@
         <c:axId val="568288208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="2.2999999999999998"/>
+          <c:min val="3"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -968,6 +967,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2832,34 +2832,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -2868,7 +2868,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
@@ -2886,7 +2886,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
@@ -2904,7 +2904,7 @@
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
@@ -2913,7 +2913,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
@@ -2922,7 +2922,7 @@
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -2931,7 +2931,7 @@
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -2940,7 +2940,7 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
@@ -2958,7 +2958,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>14</v>
       </c>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
@@ -2976,7 +2976,7 @@
       </c>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
@@ -2985,7 +2985,7 @@
       </c>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>17</v>
       </c>
@@ -2994,7 +2994,7 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>19</v>
       </c>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>20</v>
       </c>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>21</v>
       </c>
@@ -3030,7 +3030,7 @@
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>22</v>
       </c>
@@ -3039,7 +3039,7 @@
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>23</v>
       </c>
@@ -3048,7 +3048,7 @@
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>25</v>
       </c>
@@ -3066,7 +3066,7 @@
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>26</v>
       </c>
@@ -3075,7 +3075,7 @@
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>27</v>
       </c>
@@ -3084,7 +3084,7 @@
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>28</v>
       </c>
@@ -3093,7 +3093,7 @@
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>29</v>
       </c>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
@@ -3111,7 +3111,7 @@
       </c>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>31</v>
       </c>
@@ -3120,7 +3120,7 @@
       </c>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>32</v>
       </c>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>34</v>
       </c>
@@ -3147,7 +3147,7 @@
       </c>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>35</v>
       </c>
@@ -3156,7 +3156,7 @@
       </c>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>36</v>
       </c>
@@ -3165,7 +3165,7 @@
       </c>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>37</v>
       </c>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>38</v>
       </c>
@@ -3183,7 +3183,7 @@
       </c>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>39</v>
       </c>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>40</v>
       </c>
@@ -3211,20 +3211,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="9" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>49</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>47</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>33</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>35</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>44</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>6</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>25</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="36" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>41</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>45</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>26</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>3.4285714285714284</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>15</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>18</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>3.5789473684210527</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>27</v>
       </c>
@@ -3360,7 +3360,7 @@
         <v>3.7058823529411766</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>21</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>3.7142857142857144</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>30</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>19</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>3.8000000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>34</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>4.375</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>42</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>4.4259259259259256</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>16</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>20</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>29</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>36</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>32</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>4.5882352941176467</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>22</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>48</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="24" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>46</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>4.833333333333333</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>8</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>43</v>
       </c>

</xml_diff>